<commit_message>
Atualizacao 2 rodada bohry.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -905,7 +905,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J57" activeCellId="0" sqref="J57"/>
     </sheetView>
   </sheetViews>
@@ -2724,7 +2724,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K54" activeCellId="0" sqref="K54"/>
     </sheetView>
   </sheetViews>
@@ -4531,7 +4531,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
     </sheetView>
   </sheetViews>
@@ -6348,7 +6348,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -8294,7 +8294,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -10112,7 +10112,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -11930,7 +11930,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -13875,8 +13875,8 @@
   </sheetPr>
   <dimension ref="A1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I53" activeCellId="0" sqref="I53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13994,11 +13994,15 @@
       <c r="C6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G6" s="17" t="s">
         <v>7</v>
       </c>
@@ -14015,11 +14019,15 @@
       <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="17" t="s">
         <v>6</v>
       </c>
@@ -14036,11 +14044,15 @@
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="26"/>
+      <c r="F8" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" s="17" t="s">
         <v>4</v>
       </c>
@@ -14057,11 +14069,15 @@
       <c r="C9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G9" s="17" t="s">
         <v>7</v>
       </c>
@@ -14162,11 +14178,15 @@
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" s="17" t="s">
         <v>10</v>
       </c>
@@ -14183,11 +14203,15 @@
       <c r="C15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G15" s="17" t="s">
         <v>13</v>
       </c>
@@ -14204,11 +14228,15 @@
       <c r="C16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E16" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="26"/>
+      <c r="F16" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" s="17" t="s">
         <v>10</v>
       </c>
@@ -14225,11 +14253,15 @@
       <c r="C17" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E17" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="26"/>
+      <c r="F17" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G17" s="17" t="s">
         <v>12</v>
       </c>
@@ -14330,11 +14362,15 @@
       <c r="C22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G22" s="17" t="s">
         <v>16</v>
       </c>
@@ -14351,11 +14387,15 @@
       <c r="C23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G23" s="17" t="s">
         <v>17</v>
       </c>
@@ -14372,11 +14412,15 @@
       <c r="C24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G24" s="17" t="s">
         <v>15</v>
       </c>
@@ -14393,11 +14437,15 @@
       <c r="C25" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G25" s="17" t="s">
         <v>17</v>
       </c>
@@ -14498,11 +14546,15 @@
       <c r="C30" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G30" s="17" t="s">
         <v>22</v>
       </c>
@@ -14519,11 +14571,15 @@
       <c r="C31" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E31" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G31" s="17" t="s">
         <v>21</v>
       </c>
@@ -14540,11 +14596,15 @@
       <c r="C32" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E32" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G32" s="17" t="s">
         <v>22</v>
       </c>
@@ -14561,11 +14621,15 @@
       <c r="C33" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E33" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G33" s="17" t="s">
         <v>20</v>
       </c>
@@ -14668,11 +14732,15 @@
       <c r="C38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="26" t="n">
+        <v>4</v>
+      </c>
       <c r="E38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G38" s="17" t="s">
         <v>26</v>
       </c>
@@ -14689,11 +14757,15 @@
       <c r="C39" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E39" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G39" s="17" t="s">
         <v>29</v>
       </c>
@@ -14710,11 +14782,15 @@
       <c r="C40" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="26"/>
+      <c r="D40" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E40" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="26"/>
+      <c r="F40" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G40" s="17" t="s">
         <v>28</v>
       </c>
@@ -14731,11 +14807,15 @@
       <c r="C41" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="26"/>
+      <c r="D41" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E41" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="26"/>
+      <c r="F41" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G41" s="17" t="s">
         <v>26</v>
       </c>
@@ -14836,11 +14916,15 @@
       <c r="C46" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E46" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G46" s="17" t="s">
         <v>32</v>
       </c>
@@ -14857,11 +14941,15 @@
       <c r="C47" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="26"/>
+      <c r="D47" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E47" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="26"/>
+      <c r="F47" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G47" s="17" t="s">
         <v>33</v>
       </c>
@@ -14878,11 +14966,15 @@
       <c r="C48" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="26"/>
+      <c r="D48" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E48" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="26"/>
+      <c r="F48" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G48" s="17" t="s">
         <v>33</v>
       </c>
@@ -14899,11 +14991,15 @@
       <c r="C49" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="26"/>
+      <c r="D49" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="26"/>
+      <c r="F49" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G49" s="17" t="s">
         <v>31</v>
       </c>
@@ -15004,11 +15100,15 @@
       <c r="C54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="26"/>
+      <c r="D54" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E54" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="26"/>
+      <c r="F54" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G54" s="17" t="s">
         <v>38</v>
       </c>
@@ -15025,11 +15125,15 @@
       <c r="C55" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="26"/>
+      <c r="D55" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E55" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" s="17" t="s">
         <v>37</v>
       </c>
@@ -15046,11 +15150,15 @@
       <c r="C56" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="26"/>
+      <c r="D56" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E56" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="26"/>
+      <c r="F56" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G56" s="17" t="s">
         <v>36</v>
       </c>
@@ -15067,11 +15175,15 @@
       <c r="C57" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="26"/>
+      <c r="D57" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E57" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="26"/>
+      <c r="F57" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G57" s="17" t="s">
         <v>38</v>
       </c>
@@ -15168,11 +15280,15 @@
       <c r="C62" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="26"/>
+      <c r="D62" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E62" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="26"/>
+      <c r="F62" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G62" s="17" t="s">
         <v>44</v>
       </c>
@@ -15189,11 +15305,15 @@
       <c r="C63" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E63" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="26"/>
+      <c r="F63" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G63" s="17" t="s">
         <v>41</v>
       </c>
@@ -15210,11 +15330,15 @@
       <c r="C64" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="26"/>
+      <c r="D64" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E64" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="26"/>
+      <c r="F64" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G64" s="17" t="s">
         <v>43</v>
       </c>
@@ -15231,11 +15355,15 @@
       <c r="C65" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="36"/>
+      <c r="D65" s="36" t="n">
+        <v>0</v>
+      </c>
       <c r="E65" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="36"/>
+      <c r="F65" s="36" t="n">
+        <v>1</v>
+      </c>
       <c r="G65" s="35" t="s">
         <v>41</v>
       </c>
@@ -15816,7 +15944,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -17761,7 +17889,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualizacao segunda rodada - Callegas.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -905,7 +905,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J57" activeCellId="0" sqref="J57"/>
     </sheetView>
   </sheetViews>
@@ -2724,7 +2724,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K54" activeCellId="0" sqref="K54"/>
     </sheetView>
   </sheetViews>
@@ -4531,8 +4531,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4643,11 +4643,15 @@
       <c r="C6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G6" s="17" t="s">
         <v>7</v>
       </c>
@@ -4663,11 +4667,15 @@
       <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="17" t="s">
         <v>6</v>
       </c>
@@ -4801,11 +4809,15 @@
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" s="17" t="s">
         <v>10</v>
       </c>
@@ -4821,11 +4833,15 @@
       <c r="C15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G15" s="17" t="s">
         <v>13</v>
       </c>
@@ -4959,11 +4975,15 @@
       <c r="C22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G22" s="17" t="s">
         <v>16</v>
       </c>
@@ -4979,11 +4999,15 @@
       <c r="C23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G23" s="17" t="s">
         <v>17</v>
       </c>
@@ -5117,11 +5141,15 @@
       <c r="C30" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G30" s="17" t="s">
         <v>22</v>
       </c>
@@ -5137,11 +5165,15 @@
       <c r="C31" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E31" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G31" s="17" t="s">
         <v>21</v>
       </c>
@@ -5275,11 +5307,15 @@
       <c r="C38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G38" s="17" t="s">
         <v>26</v>
       </c>
@@ -5295,11 +5331,15 @@
       <c r="C39" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E39" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G39" s="17" t="s">
         <v>29</v>
       </c>
@@ -5433,11 +5473,15 @@
       <c r="C46" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E46" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G46" s="17" t="s">
         <v>32</v>
       </c>
@@ -5453,11 +5497,15 @@
       <c r="C47" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="26"/>
+      <c r="D47" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E47" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="26"/>
+      <c r="F47" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G47" s="17" t="s">
         <v>33</v>
       </c>
@@ -5591,11 +5639,15 @@
       <c r="C54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="26"/>
+      <c r="D54" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E54" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="26"/>
+      <c r="F54" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G54" s="17" t="s">
         <v>38</v>
       </c>
@@ -5611,11 +5663,15 @@
       <c r="C55" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="26"/>
+      <c r="D55" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E55" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" s="17" t="s">
         <v>37</v>
       </c>
@@ -5745,11 +5801,15 @@
       <c r="C62" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="26"/>
+      <c r="D62" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E62" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="26"/>
+      <c r="F62" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G62" s="17" t="s">
         <v>44</v>
       </c>
@@ -5765,11 +5825,15 @@
       <c r="C63" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E63" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="26"/>
+      <c r="F63" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G63" s="17" t="s">
         <v>41</v>
       </c>
@@ -6348,7 +6412,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -8294,7 +8358,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -10112,7 +10176,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -11930,7 +11994,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -13875,7 +13939,7 @@
   </sheetPr>
   <dimension ref="A1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
@@ -15944,7 +16008,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -17889,7 +17953,7 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualizacao 2 rodada victor.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -905,8 +905,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J57" activeCellId="0" sqref="J57"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G63" activeCellId="0" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1017,11 +1017,15 @@
       <c r="C6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="18" t="n">
+        <v>2</v>
+      </c>
       <c r="G6" s="17" t="s">
         <v>7</v>
       </c>
@@ -1037,11 +1041,15 @@
       <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="18" t="n">
+        <v>2</v>
+      </c>
       <c r="E7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="17" t="s">
         <v>6</v>
       </c>
@@ -1175,11 +1183,15 @@
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" s="17" t="s">
         <v>10</v>
       </c>
@@ -1195,11 +1207,15 @@
       <c r="C15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G15" s="17" t="s">
         <v>13</v>
       </c>
@@ -1333,11 +1349,15 @@
       <c r="C22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G22" s="17" t="s">
         <v>16</v>
       </c>
@@ -1353,11 +1373,15 @@
       <c r="C23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G23" s="17" t="s">
         <v>17</v>
       </c>
@@ -1491,11 +1515,15 @@
       <c r="C30" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G30" s="17" t="s">
         <v>22</v>
       </c>
@@ -1511,11 +1539,15 @@
       <c r="C31" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E31" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G31" s="17" t="s">
         <v>21</v>
       </c>
@@ -1651,11 +1683,15 @@
       <c r="C38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G38" s="17" t="s">
         <v>26</v>
       </c>
@@ -1671,11 +1707,15 @@
       <c r="C39" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E39" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G39" s="17" t="s">
         <v>29</v>
       </c>
@@ -1809,11 +1849,15 @@
       <c r="C46" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E46" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G46" s="17" t="s">
         <v>32</v>
       </c>
@@ -1829,11 +1873,15 @@
       <c r="C47" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="26"/>
+      <c r="D47" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E47" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="26"/>
+      <c r="F47" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G47" s="17" t="s">
         <v>33</v>
       </c>
@@ -1967,11 +2015,15 @@
       <c r="C54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="26"/>
+      <c r="D54" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E54" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="26"/>
+      <c r="F54" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G54" s="17" t="s">
         <v>38</v>
       </c>
@@ -1987,11 +2039,15 @@
       <c r="C55" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="26"/>
+      <c r="D55" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E55" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" s="17" t="s">
         <v>37</v>
       </c>
@@ -2121,11 +2177,15 @@
       <c r="C62" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="26"/>
+      <c r="D62" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E62" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="26"/>
+      <c r="F62" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G62" s="17" t="s">
         <v>44</v>
       </c>
@@ -2141,11 +2201,15 @@
       <c r="C63" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E63" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="26"/>
+      <c r="F63" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G63" s="17" t="s">
         <v>41</v>
       </c>
@@ -4531,7 +4595,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualizacao rodada 2 Gui.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -905,7 +905,7 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G63" activeCellId="0" sqref="G63"/>
     </sheetView>
   </sheetViews>
@@ -8422,8 +8422,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -8534,11 +8534,15 @@
       <c r="C6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="58"/>
+      <c r="D6" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="E6" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="58"/>
+      <c r="F6" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="G6" s="57" t="s">
         <v>7</v>
       </c>
@@ -8554,11 +8558,15 @@
       <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="58"/>
+      <c r="D7" s="58" t="n">
+        <v>3</v>
+      </c>
       <c r="E7" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="58"/>
+      <c r="F7" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="57" t="s">
         <v>6</v>
       </c>
@@ -8692,11 +8700,15 @@
       <c r="C14" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="58"/>
+      <c r="D14" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="E14" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="58"/>
+      <c r="F14" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" s="57" t="s">
         <v>10</v>
       </c>
@@ -8712,11 +8724,15 @@
       <c r="C15" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="58"/>
+      <c r="D15" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="E15" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="58"/>
+      <c r="F15" s="58" t="n">
+        <v>3</v>
+      </c>
       <c r="G15" s="57" t="s">
         <v>13</v>
       </c>
@@ -8850,11 +8866,15 @@
       <c r="C22" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="58"/>
+      <c r="D22" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="E22" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="58"/>
+      <c r="F22" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="G22" s="57" t="s">
         <v>16</v>
       </c>
@@ -8870,11 +8890,15 @@
       <c r="C23" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="58"/>
+      <c r="D23" s="58" t="n">
+        <v>3</v>
+      </c>
       <c r="E23" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="58"/>
+      <c r="F23" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="G23" s="57" t="s">
         <v>17</v>
       </c>
@@ -9008,11 +9032,15 @@
       <c r="C30" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="58"/>
+      <c r="D30" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="E30" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="58"/>
+      <c r="F30" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="G30" s="57" t="s">
         <v>22</v>
       </c>
@@ -9028,11 +9056,15 @@
       <c r="C31" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="58"/>
+      <c r="D31" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="E31" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="58"/>
+      <c r="F31" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="G31" s="57" t="s">
         <v>21</v>
       </c>
@@ -9168,11 +9200,15 @@
       <c r="C38" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="58"/>
+      <c r="D38" s="58" t="n">
+        <v>3</v>
+      </c>
       <c r="E38" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="58"/>
+      <c r="F38" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="G38" s="57" t="s">
         <v>26</v>
       </c>
@@ -9188,11 +9224,15 @@
       <c r="C39" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="58"/>
+      <c r="D39" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="E39" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="58"/>
+      <c r="F39" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="G39" s="57" t="s">
         <v>29</v>
       </c>
@@ -9326,11 +9366,15 @@
       <c r="C46" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="58"/>
+      <c r="D46" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="E46" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="58"/>
+      <c r="F46" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="G46" s="57" t="s">
         <v>32</v>
       </c>
@@ -9346,11 +9390,15 @@
       <c r="C47" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="58"/>
+      <c r="D47" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="E47" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="58"/>
+      <c r="F47" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="G47" s="57" t="s">
         <v>33</v>
       </c>
@@ -9484,11 +9532,15 @@
       <c r="C54" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="58"/>
+      <c r="D54" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="E54" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="58"/>
+      <c r="F54" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="G54" s="57" t="s">
         <v>38</v>
       </c>
@@ -9504,11 +9556,15 @@
       <c r="C55" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="58"/>
+      <c r="D55" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="E55" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="58"/>
+      <c r="F55" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" s="57" t="s">
         <v>37</v>
       </c>
@@ -9638,11 +9694,15 @@
       <c r="C62" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="58"/>
+      <c r="D62" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="E62" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="58"/>
+      <c r="F62" s="58" t="n">
+        <v>1</v>
+      </c>
       <c r="G62" s="57" t="s">
         <v>44</v>
       </c>
@@ -9658,11 +9718,15 @@
       <c r="C63" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="58"/>
+      <c r="D63" s="58" t="n">
+        <v>0</v>
+      </c>
       <c r="E63" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="58"/>
+      <c r="F63" s="58" t="n">
+        <v>2</v>
+      </c>
       <c r="G63" s="57" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Atualizando rodada 2 de matheus e gabriel e atualizando jogo colombia x japao.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -906,7 +906,7 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G63" activeCellId="0" sqref="G63"/>
+      <selection pane="topLeft" activeCell="H63" activeCellId="0" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2120,28 +2120,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
@@ -2788,8 +2790,8 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K54" activeCellId="0" sqref="K54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L41" activeCellId="0" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2890,11 +2892,15 @@
       <c r="C6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G6" s="17" t="s">
         <v>7</v>
       </c>
@@ -2910,11 +2916,15 @@
       <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="17" t="s">
         <v>6</v>
       </c>
@@ -3048,11 +3058,15 @@
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G14" s="17" t="s">
         <v>10</v>
       </c>
@@ -3068,11 +3082,15 @@
       <c r="C15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G15" s="17" t="s">
         <v>13</v>
       </c>
@@ -3206,11 +3224,15 @@
       <c r="C22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G22" s="17" t="s">
         <v>16</v>
       </c>
@@ -3226,11 +3248,15 @@
       <c r="C23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G23" s="17" t="s">
         <v>17</v>
       </c>
@@ -3364,11 +3390,15 @@
       <c r="C30" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G30" s="17" t="s">
         <v>22</v>
       </c>
@@ -3384,11 +3414,15 @@
       <c r="C31" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E31" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G31" s="17" t="s">
         <v>21</v>
       </c>
@@ -3524,11 +3558,15 @@
       <c r="C38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G38" s="17" t="s">
         <v>26</v>
       </c>
@@ -3544,11 +3582,15 @@
       <c r="C39" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E39" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G39" s="17" t="s">
         <v>29</v>
       </c>
@@ -3682,11 +3724,15 @@
       <c r="C46" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E46" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G46" s="17" t="s">
         <v>32</v>
       </c>
@@ -3702,11 +3748,15 @@
       <c r="C47" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="26"/>
+      <c r="D47" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E47" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="26"/>
+      <c r="F47" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G47" s="17" t="s">
         <v>33</v>
       </c>
@@ -3840,11 +3890,15 @@
       <c r="C54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="26"/>
+      <c r="D54" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E54" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="26"/>
+      <c r="F54" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G54" s="17" t="s">
         <v>38</v>
       </c>
@@ -3860,11 +3914,15 @@
       <c r="C55" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="26"/>
+      <c r="D55" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E55" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" s="17" t="s">
         <v>37</v>
       </c>
@@ -3937,28 +3995,28 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
@@ -3994,11 +4052,15 @@
       <c r="C62" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="26"/>
+      <c r="D62" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E62" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="26"/>
+      <c r="F62" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G62" s="17" t="s">
         <v>44</v>
       </c>
@@ -4014,11 +4076,15 @@
       <c r="C63" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E63" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="26"/>
+      <c r="F63" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G63" s="17" t="s">
         <v>41</v>
       </c>
@@ -4595,8 +4661,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5808,28 +5874,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
@@ -6477,7 +6545,7 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7747,28 +7815,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
@@ -8422,8 +8492,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9637,28 +9707,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="55" t="n">
+      <c r="A60" s="59" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="56" t="n">
+      <c r="B60" s="60" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="57" t="s">
+      <c r="C60" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="58" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="57" t="s">
+      <c r="D60" s="62" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="58"/>
+      <c r="H60" s="62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="55" t="n">
@@ -10304,8 +10376,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10416,11 +10488,15 @@
       <c r="C6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G6" s="17" t="s">
         <v>7</v>
       </c>
@@ -10436,11 +10512,15 @@
       <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="17" t="s">
         <v>6</v>
       </c>
@@ -10574,11 +10654,15 @@
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="26" t="n">
+        <v>4</v>
+      </c>
       <c r="E14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" s="17" t="s">
         <v>10</v>
       </c>
@@ -10594,11 +10678,15 @@
       <c r="C15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="26" t="n">
+        <v>4</v>
+      </c>
       <c r="G15" s="17" t="s">
         <v>13</v>
       </c>
@@ -10732,11 +10820,15 @@
       <c r="C22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G22" s="17" t="s">
         <v>16</v>
       </c>
@@ -10752,11 +10844,15 @@
       <c r="C23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G23" s="17" t="s">
         <v>17</v>
       </c>
@@ -10890,11 +10986,15 @@
       <c r="C30" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G30" s="17" t="s">
         <v>22</v>
       </c>
@@ -10910,11 +11010,15 @@
       <c r="C31" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E31" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G31" s="17" t="s">
         <v>21</v>
       </c>
@@ -11050,11 +11154,15 @@
       <c r="C38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="26" t="n">
+        <v>4</v>
+      </c>
       <c r="E38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G38" s="17" t="s">
         <v>26</v>
       </c>
@@ -11070,11 +11178,15 @@
       <c r="C39" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E39" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="G39" s="17" t="s">
         <v>29</v>
       </c>
@@ -11208,11 +11320,15 @@
       <c r="C46" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="E46" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G46" s="17" t="s">
         <v>32</v>
       </c>
@@ -11228,11 +11344,15 @@
       <c r="C47" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="26"/>
+      <c r="D47" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="E47" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="26"/>
+      <c r="F47" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G47" s="17" t="s">
         <v>33</v>
       </c>
@@ -11366,11 +11486,15 @@
       <c r="C54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="26"/>
+      <c r="D54" s="26" t="n">
+        <v>4</v>
+      </c>
       <c r="E54" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="26"/>
+      <c r="F54" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G54" s="17" t="s">
         <v>38</v>
       </c>
@@ -11386,11 +11510,15 @@
       <c r="C55" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="26"/>
+      <c r="D55" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E55" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" s="17" t="s">
         <v>37</v>
       </c>
@@ -11463,28 +11591,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
@@ -11520,11 +11650,15 @@
       <c r="C62" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="26"/>
+      <c r="D62" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E62" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="26"/>
+      <c r="F62" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G62" s="17" t="s">
         <v>44</v>
       </c>
@@ -11540,11 +11674,15 @@
       <c r="C63" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="E63" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="26"/>
+      <c r="F63" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="G63" s="17" t="s">
         <v>41</v>
       </c>
@@ -12123,7 +12261,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -13393,28 +13531,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
@@ -14068,7 +14208,7 @@
   <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
+      <selection pane="topLeft" activeCell="I60" activeCellId="0" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15412,30 +15552,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="69" t="n">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="72" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="70"/>
-      <c r="I60" s="27"/>
+      <c r="H60" s="73"/>
+      <c r="I60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="69" t="n">
@@ -16137,7 +16279,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17407,28 +17549,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
@@ -18082,7 +18226,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -19352,28 +19496,30 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="A60" s="5" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="16" t="n">
+      <c r="B60" s="6" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="D60" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="27"/>
+      <c r="H60" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">

</xml_diff>

<commit_message>
Adicionando jogos do gui e callegas.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -2761,8 +2761,8 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2921,11 +2921,15 @@
       <c r="C8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2941,11 +2945,15 @@
       <c r="C9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G9" s="23" t="s">
         <v>7</v>
       </c>
@@ -3091,11 +3099,15 @@
       <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" s="23" t="s">
         <v>10</v>
       </c>
@@ -3111,11 +3123,15 @@
       <c r="C17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="32"/>
+      <c r="F17" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G17" s="23" t="s">
         <v>12</v>
       </c>
@@ -3261,11 +3277,15 @@
       <c r="C24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="32"/>
+      <c r="F24" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G24" s="23" t="s">
         <v>15</v>
       </c>
@@ -3281,11 +3301,15 @@
       <c r="C25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E25" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="32"/>
+      <c r="F25" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3431,11 +3455,15 @@
       <c r="C32" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E32" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G32" s="23" t="s">
         <v>22</v>
       </c>
@@ -3451,11 +3479,15 @@
       <c r="C33" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="32"/>
+      <c r="D33" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G33" s="23" t="s">
         <v>20</v>
       </c>
@@ -3603,11 +3635,15 @@
       <c r="C40" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="32"/>
+      <c r="D40" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E40" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="32"/>
+      <c r="F40" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G40" s="23" t="s">
         <v>28</v>
       </c>
@@ -3623,11 +3659,15 @@
       <c r="C41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="32"/>
+      <c r="D41" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E41" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="32"/>
+      <c r="F41" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G41" s="23" t="s">
         <v>26</v>
       </c>
@@ -3771,11 +3811,15 @@
       <c r="C48" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="32"/>
+      <c r="D48" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E48" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="32"/>
+      <c r="F48" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G48" s="23" t="s">
         <v>33</v>
       </c>
@@ -3791,11 +3835,15 @@
       <c r="C49" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="32"/>
+      <c r="D49" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="32"/>
+      <c r="F49" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G49" s="23" t="s">
         <v>31</v>
       </c>
@@ -3941,11 +3989,15 @@
       <c r="C56" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="32"/>
+      <c r="D56" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E56" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="32"/>
+      <c r="F56" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G56" s="23" t="s">
         <v>36</v>
       </c>
@@ -3961,11 +4013,15 @@
       <c r="C57" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="32"/>
+      <c r="D57" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E57" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="32"/>
+      <c r="F57" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G57" s="23" t="s">
         <v>38</v>
       </c>
@@ -4111,11 +4167,15 @@
       <c r="C64" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="32"/>
+      <c r="D64" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E64" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="32"/>
+      <c r="F64" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G64" s="23" t="s">
         <v>43</v>
       </c>
@@ -4131,11 +4191,15 @@
       <c r="C65" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="42"/>
+      <c r="D65" s="42" t="n">
+        <v>1</v>
+      </c>
       <c r="E65" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="42"/>
+      <c r="F65" s="42" t="n">
+        <v>3</v>
+      </c>
       <c r="G65" s="41" t="s">
         <v>41</v>
       </c>
@@ -4672,8 +4736,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D69" activeCellId="0" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4839,11 +4903,15 @@
       <c r="C8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G8" s="23" t="s">
         <v>4</v>
       </c>
@@ -4859,11 +4927,15 @@
       <c r="C9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G9" s="23" t="s">
         <v>7</v>
       </c>
@@ -5009,11 +5081,15 @@
       <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" s="23" t="s">
         <v>10</v>
       </c>
@@ -5029,11 +5105,15 @@
       <c r="C17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="32"/>
+      <c r="F17" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G17" s="23" t="s">
         <v>12</v>
       </c>
@@ -5179,11 +5259,15 @@
       <c r="C24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="32"/>
+      <c r="F24" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G24" s="23" t="s">
         <v>15</v>
       </c>
@@ -5199,11 +5283,15 @@
       <c r="C25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E25" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="32"/>
+      <c r="F25" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G25" s="23" t="s">
         <v>17</v>
       </c>
@@ -5349,11 +5437,15 @@
       <c r="C32" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E32" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G32" s="23" t="s">
         <v>22</v>
       </c>
@@ -5369,11 +5461,15 @@
       <c r="C33" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="32"/>
+      <c r="D33" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G33" s="23" t="s">
         <v>20</v>
       </c>
@@ -5519,11 +5615,15 @@
       <c r="C40" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="32"/>
+      <c r="D40" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E40" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="32"/>
+      <c r="F40" s="32" t="n">
+        <v>4</v>
+      </c>
       <c r="G40" s="23" t="s">
         <v>28</v>
       </c>
@@ -5539,11 +5639,15 @@
       <c r="C41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="32"/>
+      <c r="D41" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E41" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="32"/>
+      <c r="F41" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G41" s="23" t="s">
         <v>26</v>
       </c>
@@ -5689,11 +5793,15 @@
       <c r="C48" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="32"/>
+      <c r="D48" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E48" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="32"/>
+      <c r="F48" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G48" s="23" t="s">
         <v>33</v>
       </c>
@@ -5709,11 +5817,15 @@
       <c r="C49" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="32"/>
+      <c r="D49" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="32"/>
+      <c r="F49" s="32" t="n">
+        <v>4</v>
+      </c>
       <c r="G49" s="23" t="s">
         <v>31</v>
       </c>
@@ -5859,11 +5971,15 @@
       <c r="C56" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="32"/>
+      <c r="D56" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E56" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="32"/>
+      <c r="F56" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G56" s="23" t="s">
         <v>36</v>
       </c>
@@ -5879,11 +5995,15 @@
       <c r="C57" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="32"/>
+      <c r="D57" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E57" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="32"/>
+      <c r="F57" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G57" s="23" t="s">
         <v>38</v>
       </c>
@@ -6029,11 +6149,15 @@
       <c r="C64" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="32"/>
+      <c r="D64" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E64" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="32"/>
+      <c r="F64" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G64" s="23" t="s">
         <v>43</v>
       </c>
@@ -6049,11 +6173,15 @@
       <c r="C65" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="42"/>
+      <c r="D65" s="42" t="n">
+        <v>1</v>
+      </c>
       <c r="E65" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="42"/>
+      <c r="F65" s="42" t="n">
+        <v>3</v>
+      </c>
       <c r="G65" s="41" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
update victor, gabriel e matheus.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -837,18 +837,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,11 +1006,15 @@
       <c r="C8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" s="23" t="s">
         <v>4</v>
       </c>
@@ -1026,11 +1030,15 @@
       <c r="C9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="G9" s="23" t="s">
         <v>7</v>
       </c>
@@ -1176,11 +1184,15 @@
       <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="E16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G16" s="23" t="s">
         <v>10</v>
       </c>
@@ -1196,11 +1208,15 @@
       <c r="C17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="32"/>
+      <c r="F17" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G17" s="23" t="s">
         <v>12</v>
       </c>
@@ -1346,11 +1362,15 @@
       <c r="C24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="32"/>
+      <c r="F24" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G24" s="23" t="s">
         <v>15</v>
       </c>
@@ -1366,11 +1386,15 @@
       <c r="C25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E25" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="32"/>
+      <c r="F25" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G25" s="23" t="s">
         <v>17</v>
       </c>
@@ -1516,11 +1540,15 @@
       <c r="C32" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E32" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G32" s="23" t="s">
         <v>22</v>
       </c>
@@ -1536,11 +1564,15 @@
       <c r="C33" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="32"/>
+      <c r="D33" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G33" s="23" t="s">
         <v>20</v>
       </c>
@@ -1688,11 +1720,15 @@
       <c r="C40" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="32"/>
+      <c r="D40" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E40" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="32"/>
+      <c r="F40" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G40" s="23" t="s">
         <v>28</v>
       </c>
@@ -1708,11 +1744,15 @@
       <c r="C41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="32"/>
+      <c r="D41" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E41" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="32"/>
+      <c r="F41" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G41" s="23" t="s">
         <v>26</v>
       </c>
@@ -1858,11 +1898,15 @@
       <c r="C48" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="32"/>
+      <c r="D48" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E48" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="32"/>
+      <c r="F48" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G48" s="23" t="s">
         <v>33</v>
       </c>
@@ -1878,11 +1922,15 @@
       <c r="C49" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="32"/>
+      <c r="D49" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="32"/>
+      <c r="F49" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G49" s="23" t="s">
         <v>31</v>
       </c>
@@ -2028,11 +2076,15 @@
       <c r="C56" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="32"/>
+      <c r="D56" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="E56" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="32"/>
+      <c r="F56" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G56" s="23" t="s">
         <v>36</v>
       </c>
@@ -2048,11 +2100,15 @@
       <c r="C57" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="32"/>
+      <c r="D57" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E57" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="32"/>
+      <c r="F57" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G57" s="23" t="s">
         <v>38</v>
       </c>
@@ -2198,11 +2254,15 @@
       <c r="C64" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="32"/>
+      <c r="D64" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E64" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="32"/>
+      <c r="F64" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G64" s="23" t="s">
         <v>43</v>
       </c>
@@ -2218,11 +2278,15 @@
       <c r="C65" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="42"/>
+      <c r="D65" s="42" t="n">
+        <v>2</v>
+      </c>
       <c r="E65" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="42"/>
+      <c r="F65" s="42" t="n">
+        <v>3</v>
+      </c>
       <c r="G65" s="41" t="s">
         <v>41</v>
       </c>
@@ -2746,7 +2810,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2761,16 +2825,16 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2921,11 +2985,15 @@
       <c r="C8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2941,11 +3009,15 @@
       <c r="C9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G9" s="23" t="s">
         <v>7</v>
       </c>
@@ -3091,11 +3163,15 @@
       <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" s="23" t="s">
         <v>10</v>
       </c>
@@ -3111,11 +3187,15 @@
       <c r="C17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="32"/>
+      <c r="F17" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G17" s="23" t="s">
         <v>12</v>
       </c>
@@ -3261,11 +3341,15 @@
       <c r="C24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="32"/>
+      <c r="F24" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G24" s="23" t="s">
         <v>15</v>
       </c>
@@ -3281,11 +3365,15 @@
       <c r="C25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E25" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="32"/>
+      <c r="F25" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3431,11 +3519,15 @@
       <c r="C32" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E32" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G32" s="23" t="s">
         <v>22</v>
       </c>
@@ -3451,11 +3543,15 @@
       <c r="C33" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="32"/>
+      <c r="D33" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G33" s="23" t="s">
         <v>20</v>
       </c>
@@ -3603,11 +3699,15 @@
       <c r="C40" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="32"/>
+      <c r="D40" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E40" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="32"/>
+      <c r="F40" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G40" s="23" t="s">
         <v>28</v>
       </c>
@@ -3623,11 +3723,15 @@
       <c r="C41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="32"/>
+      <c r="D41" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E41" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="32"/>
+      <c r="F41" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G41" s="23" t="s">
         <v>26</v>
       </c>
@@ -3771,11 +3875,15 @@
       <c r="C48" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="32"/>
+      <c r="D48" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E48" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="32"/>
+      <c r="F48" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G48" s="23" t="s">
         <v>33</v>
       </c>
@@ -3791,11 +3899,15 @@
       <c r="C49" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="32"/>
+      <c r="D49" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="32"/>
+      <c r="F49" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G49" s="23" t="s">
         <v>31</v>
       </c>
@@ -3941,11 +4053,15 @@
       <c r="C56" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="32"/>
+      <c r="D56" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E56" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="32"/>
+      <c r="F56" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G56" s="23" t="s">
         <v>36</v>
       </c>
@@ -3961,11 +4077,15 @@
       <c r="C57" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="32"/>
+      <c r="D57" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E57" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="32"/>
+      <c r="F57" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G57" s="23" t="s">
         <v>38</v>
       </c>
@@ -4111,11 +4231,15 @@
       <c r="C64" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="32"/>
+      <c r="D64" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E64" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="32"/>
+      <c r="F64" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G64" s="23" t="s">
         <v>43</v>
       </c>
@@ -4131,11 +4255,15 @@
       <c r="C65" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="42"/>
+      <c r="D65" s="42" t="n">
+        <v>1</v>
+      </c>
       <c r="E65" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="42"/>
+      <c r="F65" s="42" t="n">
+        <v>2</v>
+      </c>
       <c r="G65" s="41" t="s">
         <v>41</v>
       </c>
@@ -4657,7 +4785,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4670,18 +4798,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D69" activeCellId="0" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6641,7 +6769,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6654,18 +6782,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8626,7 +8754,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8639,18 +8767,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10611,7 +10739,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -10624,18 +10752,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D66" activeCellId="0" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10793,11 +10921,15 @@
       <c r="C8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G8" s="23" t="s">
         <v>4</v>
       </c>
@@ -10813,11 +10945,15 @@
       <c r="C9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G9" s="23" t="s">
         <v>7</v>
       </c>
@@ -10963,11 +11099,15 @@
       <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" s="23" t="s">
         <v>10</v>
       </c>
@@ -10983,11 +11123,15 @@
       <c r="C17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="32"/>
+      <c r="F17" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G17" s="23" t="s">
         <v>12</v>
       </c>
@@ -11133,11 +11277,15 @@
       <c r="C24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="32"/>
+      <c r="F24" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G24" s="23" t="s">
         <v>15</v>
       </c>
@@ -11153,11 +11301,15 @@
       <c r="C25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E25" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="32"/>
+      <c r="F25" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G25" s="23" t="s">
         <v>17</v>
       </c>
@@ -11303,11 +11455,15 @@
       <c r="C32" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E32" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G32" s="23" t="s">
         <v>22</v>
       </c>
@@ -11323,11 +11479,15 @@
       <c r="C33" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="32"/>
+      <c r="D33" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G33" s="23" t="s">
         <v>20</v>
       </c>
@@ -11475,11 +11635,15 @@
       <c r="C40" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="32"/>
+      <c r="D40" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E40" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="32"/>
+      <c r="F40" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="G40" s="23" t="s">
         <v>28</v>
       </c>
@@ -11495,11 +11659,15 @@
       <c r="C41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="32"/>
+      <c r="D41" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E41" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="32"/>
+      <c r="F41" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="G41" s="23" t="s">
         <v>26</v>
       </c>
@@ -11645,11 +11813,15 @@
       <c r="C48" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="32"/>
+      <c r="D48" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E48" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="32"/>
+      <c r="F48" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G48" s="23" t="s">
         <v>33</v>
       </c>
@@ -11665,11 +11837,15 @@
       <c r="C49" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="32"/>
+      <c r="D49" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="32"/>
+      <c r="F49" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G49" s="23" t="s">
         <v>31</v>
       </c>
@@ -11815,11 +11991,15 @@
       <c r="C56" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="32"/>
+      <c r="D56" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="E56" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="32"/>
+      <c r="F56" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="G56" s="23" t="s">
         <v>36</v>
       </c>
@@ -11835,11 +12015,15 @@
       <c r="C57" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="32"/>
+      <c r="D57" s="32" t="n">
+        <v>0</v>
+      </c>
       <c r="E57" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="32"/>
+      <c r="F57" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G57" s="23" t="s">
         <v>38</v>
       </c>
@@ -11985,11 +12169,15 @@
       <c r="C64" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="32"/>
+      <c r="D64" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="E64" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="32"/>
+      <c r="F64" s="32" t="n">
+        <v>1</v>
+      </c>
       <c r="G64" s="23" t="s">
         <v>43</v>
       </c>
@@ -12005,11 +12193,15 @@
       <c r="C65" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="42"/>
+      <c r="D65" s="42" t="n">
+        <v>2</v>
+      </c>
       <c r="E65" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="42"/>
+      <c r="F65" s="42" t="n">
+        <v>3</v>
+      </c>
       <c r="G65" s="41" t="s">
         <v>41</v>
       </c>
@@ -12532,7 +12724,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -12547,16 +12739,16 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14516,7 +14708,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14531,16 +14723,16 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H66" activeCellId="0" sqref="H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16500,7 +16692,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -16515,16 +16707,16 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H65" activeCellId="0" sqref="H65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18487,7 +18679,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -18502,16 +18694,16 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H65" activeCellId="0" sqref="H65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20471,7 +20663,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
correcoes belgica x inglaterra e tunisia x panama.
</commit_message>
<xml_diff>
--- a/bolão final 1 rodada.xlsx
+++ b/bolão final 1 rodada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="73">
   <si>
     <t xml:space="preserve">RESULTADOS</t>
   </si>
@@ -232,10 +232,13 @@
     <t xml:space="preserve">PALPITE DO CAMPEÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">França </t>
+    <t xml:space="preserve">Suecia</t>
   </si>
   <si>
     <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">França </t>
   </si>
   <si>
     <t xml:space="preserve">Croacia</t>
@@ -476,7 +479,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -669,6 +672,54 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
@@ -844,8 +895,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H74" activeCellId="0" sqref="H74"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -878,7 +929,7 @@
       <c r="G2" s="0"/>
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2168,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -2141,7 +2194,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -2906,8 +2961,8 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C43" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R38" activeCellId="0" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2933,7 +2988,7 @@
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4108,19 +4163,19 @@
       <c r="C54" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="70" t="n">
+      <c r="D54" s="82" t="n">
         <v>2</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="70" t="n">
+      <c r="F54" s="82" t="n">
         <v>1</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H54" s="71" t="n">
+      <c r="H54" s="83" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4134,19 +4189,19 @@
       <c r="C55" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="70" t="n">
+      <c r="D55" s="82" t="n">
         <v>2</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="70" t="n">
+      <c r="F55" s="82" t="n">
         <v>0</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H55" s="71" t="n">
+      <c r="H55" s="83" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4172,7 +4227,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -4196,7 +4253,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -4959,8 +5018,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N42" activeCellId="0" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4993,7 +5052,7 @@
       <c r="G2" s="0"/>
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5845,54 +5904,54 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="32" t="n">
+      <c r="A40" s="11" t="n">
         <v>43278</v>
       </c>
-      <c r="B40" s="33" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C40" s="34" t="s">
+      <c r="B40" s="12" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="35" t="n">
+      <c r="D40" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="G40" s="34" t="s">
+      <c r="G40" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="36" t="n">
+      <c r="H40" s="15" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="32" t="n">
+      <c r="A41" s="6" t="n">
         <v>43278</v>
       </c>
-      <c r="B41" s="33" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C41" s="34" t="s">
+      <c r="B41" s="7" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="34" t="s">
+      <c r="D41" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H41" s="36" t="n">
+      <c r="H41" s="10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6027,54 +6086,54 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="32" t="n">
+      <c r="A48" s="6" t="n">
         <v>43278</v>
       </c>
-      <c r="B48" s="33" t="n">
+      <c r="B48" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="E48" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F48" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="G48" s="34" t="s">
+      <c r="D48" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H48" s="36" t="n">
+      <c r="H48" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="32" t="n">
+      <c r="A49" s="6" t="n">
         <v>43278</v>
       </c>
-      <c r="B49" s="33" t="n">
+      <c r="B49" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="35" t="n">
+      <c r="D49" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="G49" s="34" t="s">
+      <c r="G49" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H49" s="36" t="n">
+      <c r="H49" s="10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6209,52 +6268,56 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="32" t="n">
+      <c r="A56" s="11" t="n">
         <v>43279</v>
       </c>
-      <c r="B56" s="33" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C56" s="34" t="s">
+      <c r="B56" s="12" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="E56" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F56" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="G56" s="34" t="s">
+      <c r="D56" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G56" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="15" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="32" t="n">
+      <c r="A57" s="11" t="n">
         <v>43279</v>
       </c>
-      <c r="B57" s="33" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C57" s="34" t="s">
+      <c r="B57" s="12" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F57" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="G57" s="34" t="s">
+      <c r="D57" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G57" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="15" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -6335,28 +6398,28 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="32" t="n">
+      <c r="A62" s="6" t="n">
         <v>43275</v>
       </c>
-      <c r="B62" s="33" t="n">
+      <c r="B62" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="C62" s="34" t="s">
+      <c r="C62" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="E62" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" s="34" t="s">
+      <c r="D62" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H62" s="36" t="n">
+      <c r="H62" s="10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6387,54 +6450,54 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="32" t="n">
+      <c r="A64" s="6" t="n">
         <v>43279</v>
       </c>
-      <c r="B64" s="33" t="n">
+      <c r="B64" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C64" s="34" t="s">
+      <c r="C64" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="E64" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F64" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" s="34" t="s">
+      <c r="D64" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H64" s="36" t="n">
+      <c r="H64" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="37" t="n">
+      <c r="A65" s="48" t="n">
         <v>43279</v>
       </c>
-      <c r="B65" s="38" t="n">
+      <c r="B65" s="49" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C65" s="39" t="s">
+      <c r="C65" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E65" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" s="40" t="n">
-        <v>3</v>
-      </c>
-      <c r="G65" s="39" t="s">
+      <c r="D65" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="G65" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="H65" s="36" t="n">
+      <c r="H65" s="15" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6465,210 +6528,210 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="32" t="n">
+      <c r="A68" s="6" t="n">
         <v>43281</v>
       </c>
-      <c r="B68" s="33" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C68" s="42" t="s">
+      <c r="B68" s="7" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C68" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D68" s="43" t="n">
-        <v>1</v>
-      </c>
-      <c r="E68" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" s="43" t="n">
-        <v>2</v>
-      </c>
-      <c r="G68" s="42" t="s">
+      <c r="D68" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="H68" s="36" t="n">
+      <c r="H68" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="32" t="n">
+      <c r="A69" s="6" t="n">
         <v>43281</v>
       </c>
-      <c r="B69" s="33" t="n">
+      <c r="B69" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C69" s="42" t="s">
+      <c r="C69" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="43" t="n">
-        <v>2</v>
-      </c>
-      <c r="E69" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" s="43" t="n">
-        <v>2</v>
-      </c>
-      <c r="G69" s="42" t="s">
+      <c r="D69" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G69" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="36" t="n">
+      <c r="H69" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="32" t="n">
+      <c r="A70" s="6" t="n">
         <v>43282</v>
       </c>
-      <c r="B70" s="33" t="n">
+      <c r="B70" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C70" s="42" t="s">
+      <c r="C70" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D70" s="43" t="n">
-        <v>3</v>
-      </c>
-      <c r="E70" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F70" s="43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G70" s="42" t="s">
+      <c r="D70" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="H70" s="36" t="n">
+      <c r="H70" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="32" t="n">
+      <c r="A71" s="6" t="n">
         <v>43282</v>
       </c>
-      <c r="B71" s="33" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C71" s="42" t="s">
+      <c r="B71" s="7" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C71" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D71" s="43" t="n">
-        <v>2</v>
-      </c>
-      <c r="E71" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" s="43" t="n">
-        <v>0</v>
-      </c>
-      <c r="G71" s="42" t="s">
+      <c r="D71" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H71" s="36" t="n">
+      <c r="H71" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="32" t="n">
+      <c r="A72" s="11" t="n">
         <v>43283</v>
       </c>
-      <c r="B72" s="33" t="n">
+      <c r="B72" s="12" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C72" s="42" t="s">
+      <c r="C72" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D72" s="43" t="n">
-        <v>2</v>
-      </c>
-      <c r="E72" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F72" s="43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G72" s="42" t="s">
+      <c r="D72" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="H72" s="36" t="n">
+      <c r="H72" s="15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="37" t="n">
+      <c r="A73" s="48" t="n">
         <v>43283</v>
       </c>
-      <c r="B73" s="38" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C73" s="44" t="s">
+      <c r="B73" s="49" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C73" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D73" s="45" t="n">
-        <v>3</v>
-      </c>
-      <c r="E73" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F73" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G73" s="44" t="s">
+      <c r="D73" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E73" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="H73" s="36" t="n">
+      <c r="H73" s="15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="37" t="n">
+      <c r="A74" s="48" t="n">
         <v>43284</v>
       </c>
-      <c r="B74" s="38" t="n">
+      <c r="B74" s="49" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C74" s="44" t="s">
+      <c r="C74" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D74" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="E74" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F74" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G74" s="44" t="s">
+      <c r="D74" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="H74" s="36" t="n">
+      <c r="H74" s="15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="37" t="n">
+      <c r="A75" s="55" t="n">
         <v>43284</v>
       </c>
-      <c r="B75" s="38" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C75" s="44" t="s">
+      <c r="B75" s="56" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C75" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D75" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="E75" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F75" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G75" s="44" t="s">
+      <c r="D75" s="58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="36" t="n">
+      <c r="H75" s="10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6705,16 +6768,16 @@
       <c r="B78" s="33" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C78" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D78" s="35"/>
+      <c r="C78" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="43"/>
       <c r="E78" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F78" s="35"/>
-      <c r="G78" s="46" t="s">
-        <v>48</v>
+      <c r="F78" s="43"/>
+      <c r="G78" s="42" t="s">
+        <v>15</v>
       </c>
       <c r="H78" s="36"/>
     </row>
@@ -6725,16 +6788,16 @@
       <c r="B79" s="33" t="n">
         <v>0.625</v>
       </c>
-      <c r="C79" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="35"/>
+      <c r="C79" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" s="43"/>
       <c r="E79" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="35"/>
-      <c r="G79" s="46" t="s">
-        <v>50</v>
+      <c r="F79" s="43"/>
+      <c r="G79" s="42" t="s">
+        <v>36</v>
       </c>
       <c r="H79" s="36"/>
     </row>
@@ -6745,16 +6808,16 @@
       <c r="B80" s="33" t="n">
         <v>0.625</v>
       </c>
-      <c r="C80" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="35"/>
+      <c r="C80" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D80" s="43"/>
       <c r="E80" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F80" s="35"/>
-      <c r="G80" s="46" t="s">
-        <v>52</v>
+      <c r="F80" s="43"/>
+      <c r="G80" s="42" t="s">
+        <v>39</v>
       </c>
       <c r="H80" s="36"/>
     </row>
@@ -6765,16 +6828,16 @@
       <c r="B81" s="33" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C81" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="D81" s="35"/>
+      <c r="C81" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D81" s="43"/>
       <c r="E81" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F81" s="35"/>
-      <c r="G81" s="46" t="s">
-        <v>54</v>
+      <c r="F81" s="43"/>
+      <c r="G81" s="42" t="s">
+        <v>22</v>
       </c>
       <c r="H81" s="36"/>
     </row>
@@ -7020,7 +7083,7 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H75" activeCellId="0" sqref="H75"/>
+      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7053,7 +7116,7 @@
       <c r="G2" s="0"/>
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8292,7 +8355,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -8316,7 +8381,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -9080,8 +9147,8 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H76" activeCellId="0" sqref="H76"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9114,178 +9181,178 @@
       <c r="G2" s="0"/>
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48" t="s">
+      <c r="A3" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="49" t="n">
+      <c r="A4" s="61" t="n">
         <v>43265</v>
       </c>
-      <c r="B4" s="50" t="n">
+      <c r="B4" s="62" t="n">
         <v>0.5</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="51" t="s">
+      <c r="D4" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="52" t="n">
+      <c r="H4" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="49" t="n">
+      <c r="A5" s="61" t="n">
         <v>43266</v>
       </c>
-      <c r="B5" s="50" t="n">
+      <c r="B5" s="62" t="n">
         <v>0.375</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="51" t="s">
+      <c r="D5" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="52" t="n">
+      <c r="H5" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="53" t="n">
+      <c r="A6" s="65" t="n">
         <v>43270</v>
       </c>
-      <c r="B6" s="54" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C6" s="55" t="s">
+      <c r="B6" s="66" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C6" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="55" t="s">
+      <c r="D6" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="56" t="n">
+      <c r="H6" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="49" t="n">
+      <c r="A7" s="61" t="n">
         <v>43271</v>
       </c>
-      <c r="B7" s="50" t="n">
+      <c r="B7" s="62" t="n">
         <v>0.5</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="51" t="s">
+      <c r="D7" s="64" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="52" t="n">
+      <c r="H7" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="49" t="n">
+      <c r="A8" s="61" t="n">
         <v>43276</v>
       </c>
-      <c r="B8" s="50" t="n">
+      <c r="B8" s="62" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="51" t="s">
+      <c r="D8" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="52" t="n">
+      <c r="H8" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53" t="n">
+      <c r="A9" s="65" t="n">
         <v>43276</v>
       </c>
-      <c r="B9" s="54" t="n">
+      <c r="B9" s="66" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="56" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" s="55" t="s">
+      <c r="D9" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="68" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="56" t="n">
+      <c r="H9" s="68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9316,158 +9383,158 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="53" t="n">
+      <c r="A12" s="65" t="n">
         <v>43266</v>
       </c>
-      <c r="B12" s="54" t="n">
+      <c r="B12" s="66" t="n">
         <v>0.5</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="55" t="s">
+      <c r="D12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="56" t="n">
+      <c r="H12" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="53" t="n">
+      <c r="A13" s="65" t="n">
         <v>43266</v>
       </c>
-      <c r="B13" s="54" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C13" s="55" t="s">
+      <c r="B13" s="66" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C13" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="55" t="s">
+      <c r="D13" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="56" t="n">
+      <c r="H13" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49" t="n">
+      <c r="A14" s="61" t="n">
         <v>43271</v>
       </c>
-      <c r="B14" s="50" t="n">
+      <c r="B14" s="62" t="n">
         <v>0.375</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="51" t="s">
+      <c r="D14" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="52" t="n">
+      <c r="H14" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="49" t="n">
+      <c r="A15" s="61" t="n">
         <v>43271</v>
       </c>
-      <c r="B15" s="50" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C15" s="51" t="s">
+      <c r="B15" s="62" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C15" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="52" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="51" t="s">
+      <c r="D15" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="64" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="52" t="n">
+      <c r="H15" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="53" t="n">
+      <c r="A16" s="65" t="n">
         <v>43276</v>
       </c>
-      <c r="B16" s="54" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C16" s="55" t="s">
+      <c r="B16" s="66" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C16" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="55" t="s">
+      <c r="D16" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="56" t="n">
+      <c r="H16" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="53" t="n">
+      <c r="A17" s="65" t="n">
         <v>43276</v>
       </c>
-      <c r="B17" s="54" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C17" s="55" t="s">
+      <c r="B17" s="66" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C17" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="56" t="n">
-        <v>3</v>
-      </c>
-      <c r="G17" s="55" t="s">
+      <c r="D17" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="68" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="56" t="n">
+      <c r="H17" s="68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9498,158 +9565,158 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="49" t="n">
+      <c r="A20" s="61" t="n">
         <v>43267</v>
       </c>
-      <c r="B20" s="50" t="n">
+      <c r="B20" s="62" t="n">
         <v>0.291666666666667</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="52" t="n">
-        <v>3</v>
-      </c>
-      <c r="E20" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="51" t="s">
+      <c r="D20" s="64" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="52" t="n">
+      <c r="H20" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53" t="n">
+      <c r="A21" s="65" t="n">
         <v>43267</v>
       </c>
-      <c r="B21" s="54" t="n">
+      <c r="B21" s="66" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="55" t="s">
+      <c r="D21" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="56" t="n">
+      <c r="H21" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="53" t="n">
+      <c r="A22" s="65" t="n">
         <v>43272</v>
       </c>
-      <c r="B22" s="54" t="n">
+      <c r="B22" s="66" t="n">
         <v>0.375</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="55" t="s">
+      <c r="D22" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="56" t="n">
+      <c r="H22" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="49" t="n">
+      <c r="A23" s="61" t="n">
         <v>43272</v>
       </c>
-      <c r="B23" s="50" t="n">
+      <c r="B23" s="62" t="n">
         <v>0.5</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="52" t="n">
-        <v>3</v>
-      </c>
-      <c r="E23" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="51" t="s">
+      <c r="D23" s="64" t="n">
+        <v>3</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="52" t="n">
+      <c r="H23" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="53" t="n">
+      <c r="A24" s="65" t="n">
         <v>43277</v>
       </c>
-      <c r="B24" s="54" t="n">
+      <c r="B24" s="66" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="55" t="s">
+      <c r="D24" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="56" t="n">
+      <c r="H24" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="53" t="n">
+      <c r="A25" s="65" t="n">
         <v>43277</v>
       </c>
-      <c r="B25" s="54" t="n">
+      <c r="B25" s="66" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="55" t="s">
+      <c r="D25" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="56" t="n">
+      <c r="H25" s="68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9680,158 +9747,158 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="53" t="n">
+      <c r="A28" s="65" t="n">
         <v>43267</v>
       </c>
-      <c r="B28" s="54" t="n">
+      <c r="B28" s="66" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="56" t="n">
+      <c r="D28" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="E28" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="55" t="s">
+      <c r="E28" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="56" t="n">
+      <c r="H28" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="57" t="n">
+      <c r="A29" s="69" t="n">
         <v>43267</v>
       </c>
-      <c r="B29" s="58" t="n">
+      <c r="B29" s="70" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="C29" s="59" t="s">
+      <c r="C29" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="60" t="n">
-        <v>2</v>
-      </c>
-      <c r="E29" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="59" t="s">
+      <c r="D29" s="72" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="60" t="n">
+      <c r="H29" s="72" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="53" t="n">
+      <c r="A30" s="65" t="n">
         <v>43272</v>
       </c>
-      <c r="B30" s="54" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C30" s="55" t="s">
+      <c r="B30" s="66" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C30" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="55" t="s">
+      <c r="D30" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="56" t="n">
+      <c r="H30" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="53" t="n">
+      <c r="A31" s="65" t="n">
         <v>43273</v>
       </c>
-      <c r="B31" s="54" t="n">
+      <c r="B31" s="66" t="n">
         <v>0.5</v>
       </c>
-      <c r="C31" s="55" t="s">
+      <c r="C31" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="55" t="s">
+      <c r="D31" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="56" t="n">
+      <c r="H31" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="49" t="n">
+      <c r="A32" s="61" t="n">
         <v>43277</v>
       </c>
-      <c r="B32" s="50" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C32" s="51" t="s">
+      <c r="B32" s="62" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C32" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="51" t="s">
+      <c r="D32" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="52" t="n">
+      <c r="H32" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="57" t="n">
+      <c r="A33" s="69" t="n">
         <v>43277</v>
       </c>
-      <c r="B33" s="58" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C33" s="59" t="s">
+      <c r="B33" s="70" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C33" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="60" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="60" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="59" t="s">
+      <c r="D33" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="72" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="60" t="n">
+      <c r="H33" s="72" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9864,158 +9931,158 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="53" t="n">
+      <c r="A36" s="65" t="n">
         <v>43268</v>
       </c>
-      <c r="B36" s="54" t="n">
+      <c r="B36" s="66" t="n">
         <v>0.375</v>
       </c>
-      <c r="C36" s="55" t="s">
+      <c r="C36" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="E36" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="55" t="s">
+      <c r="D36" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="56" t="n">
+      <c r="H36" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="53" t="n">
+      <c r="A37" s="65" t="n">
         <v>43268</v>
       </c>
-      <c r="B37" s="54" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C37" s="55" t="s">
+      <c r="B37" s="66" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C37" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="56" t="n">
+      <c r="D37" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="E37" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G37" s="55" t="s">
+      <c r="E37" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H37" s="56" t="n">
+      <c r="H37" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="49" t="n">
+      <c r="A38" s="61" t="n">
         <v>43273</v>
       </c>
-      <c r="B38" s="50" t="n">
+      <c r="B38" s="62" t="n">
         <v>0.375</v>
       </c>
-      <c r="C38" s="51" t="s">
+      <c r="C38" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="52" t="n">
-        <v>3</v>
-      </c>
-      <c r="E38" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="51" t="s">
+      <c r="D38" s="64" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="52" t="n">
+      <c r="H38" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="53" t="n">
+      <c r="A39" s="65" t="n">
         <v>43273</v>
       </c>
-      <c r="B39" s="54" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C39" s="55" t="s">
+      <c r="B39" s="66" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C39" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="55" t="s">
+      <c r="D39" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H39" s="56" t="n">
+      <c r="H39" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="61" t="n">
+      <c r="A40" s="73" t="n">
         <v>43278</v>
       </c>
-      <c r="B40" s="62" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C40" s="63" t="s">
+      <c r="B40" s="74" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C40" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="64" t="n">
-        <v>2</v>
-      </c>
-      <c r="G40" s="63" t="s">
+      <c r="D40" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="76" t="n">
+        <v>2</v>
+      </c>
+      <c r="G40" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="64" t="n">
+      <c r="H40" s="76" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="61" t="n">
+      <c r="A41" s="73" t="n">
         <v>43278</v>
       </c>
-      <c r="B41" s="62" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C41" s="63" t="s">
+      <c r="B41" s="74" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C41" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="63" t="s">
+      <c r="D41" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H41" s="64" t="n">
+      <c r="H41" s="76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10046,158 +10113,158 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="53" t="n">
+      <c r="A44" s="65" t="n">
         <v>43268</v>
       </c>
-      <c r="B44" s="54" t="n">
+      <c r="B44" s="66" t="n">
         <v>0.5</v>
       </c>
-      <c r="C44" s="55" t="s">
+      <c r="C44" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="56" t="n">
+      <c r="D44" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="E44" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F44" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G44" s="55" t="s">
+      <c r="E44" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="H44" s="56" t="n">
+      <c r="H44" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="57" t="n">
+      <c r="A45" s="69" t="n">
         <v>43269</v>
       </c>
-      <c r="B45" s="58" t="n">
+      <c r="B45" s="70" t="n">
         <v>0.375</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="60" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="59" t="s">
+      <c r="D45" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="H45" s="60" t="n">
+      <c r="H45" s="72" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="49" t="n">
+      <c r="A46" s="61" t="n">
         <v>43274</v>
       </c>
-      <c r="B46" s="50" t="n">
+      <c r="B46" s="62" t="n">
         <v>0.5</v>
       </c>
-      <c r="C46" s="51" t="s">
+      <c r="C46" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F46" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G46" s="51" t="s">
+      <c r="D46" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G46" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="H46" s="52" t="n">
+      <c r="H46" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="49" t="n">
+      <c r="A47" s="61" t="n">
         <v>43274</v>
       </c>
-      <c r="B47" s="50" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C47" s="51" t="s">
+      <c r="B47" s="62" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C47" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="E47" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F47" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" s="51" t="s">
+      <c r="D47" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="H47" s="52" t="n">
+      <c r="H47" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="61" t="n">
+      <c r="A48" s="73" t="n">
         <v>43278</v>
       </c>
-      <c r="B48" s="62" t="n">
+      <c r="B48" s="74" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C48" s="63" t="s">
+      <c r="C48" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F48" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" s="63" t="s">
+      <c r="D48" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="H48" s="64" t="n">
+      <c r="H48" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="61" t="n">
+      <c r="A49" s="73" t="n">
         <v>43278</v>
       </c>
-      <c r="B49" s="62" t="n">
+      <c r="B49" s="74" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C49" s="63" t="s">
+      <c r="C49" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="64" t="n">
-        <v>3</v>
-      </c>
-      <c r="G49" s="63" t="s">
+      <c r="D49" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="76" t="n">
+        <v>3</v>
+      </c>
+      <c r="G49" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="H49" s="64" t="n">
+      <c r="H49" s="76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10228,156 +10295,160 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="49" t="n">
+      <c r="A52" s="61" t="n">
         <v>43269</v>
       </c>
-      <c r="B52" s="50" t="n">
+      <c r="B52" s="62" t="n">
         <v>0.5</v>
       </c>
-      <c r="C52" s="51" t="s">
+      <c r="C52" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="52" t="n">
+      <c r="D52" s="64" t="n">
         <v>4</v>
       </c>
-      <c r="E52" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" s="51" t="s">
+      <c r="E52" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="H52" s="52" t="n">
+      <c r="H52" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="49" t="n">
+      <c r="A53" s="61" t="n">
         <v>43269</v>
       </c>
-      <c r="B53" s="50" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C53" s="51" t="s">
+      <c r="B53" s="62" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C53" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D53" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F53" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G53" s="51" t="s">
+      <c r="D53" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="H53" s="52" t="n">
+      <c r="H53" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="49" t="n">
+      <c r="A54" s="61" t="n">
         <v>43274</v>
       </c>
-      <c r="B54" s="50" t="n">
+      <c r="B54" s="62" t="n">
         <v>0.375</v>
       </c>
-      <c r="C54" s="51" t="s">
+      <c r="C54" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="E54" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" s="51" t="s">
+      <c r="D54" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E54" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H54" s="52" t="n">
+      <c r="H54" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="49" t="n">
+      <c r="A55" s="61" t="n">
         <v>43275</v>
       </c>
-      <c r="B55" s="50" t="n">
+      <c r="B55" s="62" t="n">
         <v>0.375</v>
       </c>
-      <c r="C55" s="51" t="s">
+      <c r="C55" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F55" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" s="51" t="s">
+      <c r="D55" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="H55" s="52" t="n">
+      <c r="H55" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="61" t="n">
+      <c r="A56" s="73" t="n">
         <v>43279</v>
       </c>
-      <c r="B56" s="62" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C56" s="63" t="s">
+      <c r="B56" s="74" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C56" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="64" t="n">
-        <v>2</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F56" s="64" t="n">
-        <v>2</v>
-      </c>
-      <c r="G56" s="63" t="s">
+      <c r="D56" s="76" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="76" t="n">
+        <v>2</v>
+      </c>
+      <c r="G56" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="64"/>
+      <c r="H56" s="76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="61" t="n">
+      <c r="A57" s="73" t="n">
         <v>43279</v>
       </c>
-      <c r="B57" s="62" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C57" s="63" t="s">
+      <c r="B57" s="74" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C57" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F57" s="64" t="n">
-        <v>2</v>
-      </c>
-      <c r="G57" s="63" t="s">
+      <c r="D57" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" s="76" t="n">
+        <v>2</v>
+      </c>
+      <c r="G57" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="64"/>
+      <c r="H57" s="76" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -10406,158 +10477,158 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="53" t="n">
+      <c r="A60" s="65" t="n">
         <v>43270</v>
       </c>
-      <c r="B60" s="54" t="n">
+      <c r="B60" s="66" t="n">
         <v>0.375</v>
       </c>
-      <c r="C60" s="55" t="s">
+      <c r="C60" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="56" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="55" t="s">
+      <c r="D60" s="68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="56" t="n">
+      <c r="H60" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="53" t="n">
+      <c r="A61" s="65" t="n">
         <v>43270</v>
       </c>
-      <c r="B61" s="54" t="n">
+      <c r="B61" s="66" t="n">
         <v>0.5</v>
       </c>
-      <c r="C61" s="55" t="s">
+      <c r="C61" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="D61" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E61" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F61" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G61" s="55" t="s">
+      <c r="D61" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="H61" s="56" t="n">
+      <c r="H61" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="53" t="n">
+      <c r="A62" s="65" t="n">
         <v>43275</v>
       </c>
-      <c r="B62" s="54" t="n">
+      <c r="B62" s="66" t="n">
         <v>0.5</v>
       </c>
-      <c r="C62" s="55" t="s">
+      <c r="C62" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E62" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="G62" s="55" t="s">
+      <c r="D62" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="H62" s="56" t="n">
+      <c r="H62" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="49" t="n">
+      <c r="A63" s="61" t="n">
         <v>43275</v>
       </c>
-      <c r="B63" s="50" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="C63" s="51" t="s">
+      <c r="B63" s="62" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C63" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F63" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G63" s="51" t="s">
+      <c r="D63" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G63" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H63" s="52" t="n">
+      <c r="H63" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="61" t="n">
+      <c r="A64" s="73" t="n">
         <v>43279</v>
       </c>
-      <c r="B64" s="62" t="n">
+      <c r="B64" s="74" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C64" s="63" t="s">
+      <c r="C64" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="E64" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F64" s="64" t="n">
-        <v>2</v>
-      </c>
-      <c r="G64" s="63" t="s">
+      <c r="D64" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="76" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="H64" s="64" t="n">
+      <c r="H64" s="76" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="61" t="n">
+      <c r="A65" s="73" t="n">
         <v>43279</v>
       </c>
-      <c r="B65" s="62" t="n">
+      <c r="B65" s="74" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C65" s="63" t="s">
+      <c r="C65" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="E65" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" s="64" t="n">
-        <v>3</v>
-      </c>
-      <c r="G65" s="63" t="s">
+      <c r="D65" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="76" t="n">
+        <v>3</v>
+      </c>
+      <c r="G65" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="H65" s="64" t="n">
+      <c r="H65" s="76" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11142,7 +11213,7 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H76" activeCellId="0" sqref="H76"/>
+      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -11175,7 +11246,7 @@
       <c r="G2" s="0"/>
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12414,7 +12485,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -12438,7 +12511,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -12655,19 +12730,19 @@
       <c r="B68" s="33" t="n">
         <v>0.625</v>
       </c>
-      <c r="C68" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="D68" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="E68" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="G68" s="65" t="s">
+      <c r="C68" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" s="77" t="s">
         <v>20</v>
       </c>
       <c r="H68" s="36" t="n">
@@ -12681,19 +12756,19 @@
       <c r="B69" s="33" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C69" s="65" t="s">
+      <c r="C69" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E69" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="G69" s="65" t="s">
+      <c r="D69" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E69" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" s="77" t="s">
         <v>12</v>
       </c>
       <c r="H69" s="36" t="n">
@@ -12707,19 +12782,19 @@
       <c r="B70" s="33" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C70" s="65" t="s">
+      <c r="C70" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D70" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E70" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F70" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="G70" s="65" t="s">
+      <c r="D70" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" s="77" t="s">
         <v>68</v>
       </c>
       <c r="H70" s="36" t="n">
@@ -12733,19 +12808,19 @@
       <c r="B71" s="33" t="n">
         <v>0.625</v>
       </c>
-      <c r="C71" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E71" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="G71" s="65" t="s">
+      <c r="C71" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="D71" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="77" t="s">
         <v>18</v>
       </c>
       <c r="H71" s="36" t="n">
@@ -12759,19 +12834,19 @@
       <c r="B72" s="33" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C72" s="65" t="s">
+      <c r="C72" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="D72" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E72" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="F72" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" s="65" t="s">
+      <c r="D72" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" s="77" t="s">
         <v>32</v>
       </c>
       <c r="H72" s="36" t="n">
@@ -12785,19 +12860,19 @@
       <c r="B73" s="38" t="n">
         <v>0.625</v>
       </c>
-      <c r="C73" s="65" t="s">
+      <c r="C73" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="D73" s="66" t="n">
-        <v>3</v>
-      </c>
-      <c r="E73" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F73" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="G73" s="65" t="s">
+      <c r="D73" s="78" t="n">
+        <v>3</v>
+      </c>
+      <c r="E73" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" s="78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" s="77" t="s">
         <v>42</v>
       </c>
       <c r="H73" s="36" t="n">
@@ -12811,20 +12886,20 @@
       <c r="B74" s="38" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C74" s="65" t="s">
+      <c r="C74" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D74" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E74" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F74" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="G74" s="65" t="s">
-        <v>71</v>
+      <c r="D74" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" s="77" t="s">
+        <v>72</v>
       </c>
       <c r="H74" s="36" t="n">
         <v>6</v>
@@ -12837,19 +12912,19 @@
       <c r="B75" s="38" t="n">
         <v>0.625</v>
       </c>
-      <c r="C75" s="65" t="s">
+      <c r="C75" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="D75" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="E75" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F75" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="G75" s="65" t="s">
+      <c r="D75" s="78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="G75" s="77" t="s">
         <v>39</v>
       </c>
       <c r="H75" s="36" t="n">
@@ -13202,8 +13277,8 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -13889,19 +13964,19 @@
       <c r="C31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="68" t="n">
+      <c r="D31" s="80" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="68" t="n">
+      <c r="F31" s="80" t="n">
         <v>0</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="69" t="n">
+      <c r="H31" s="81" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14475,7 +14550,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -14499,7 +14576,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -15262,8 +15341,8 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15296,7 +15375,7 @@
       <c r="G2" s="0"/>
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16535,7 +16614,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -16559,7 +16640,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -17322,8 +17405,8 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J75" activeCellId="0" sqref="J75"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -18598,7 +18681,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -18622,7 +18707,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
@@ -19386,7 +19473,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
+      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -19419,7 +19506,7 @@
       <c r="G2" s="0"/>
       <c r="H2" s="3" t="n">
         <f aca="false">SUM(H4:H77)</f>
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20658,7 +20745,9 @@
       <c r="G56" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32" t="n">
@@ -20682,7 +20771,9 @@
       <c r="G57" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>

</xml_diff>